<commit_message>
feat: import jp per pekan excel
</commit_message>
<xml_diff>
--- a/public/templates/template_mapel.xlsx
+++ b/public/templates/template_mapel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ridzimeko\Documents\Projects\jadwal-azmania\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9F17311-C9A8-4763-B418-AD7DF00589D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D32587-FDFA-4163-A843-205CF9E3AC28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2865FED8-1D15-40F6-8E78-7F59FD911D5F}"/>
+    <workbookView xWindow="3330" yWindow="1620" windowWidth="15240" windowHeight="9300" xr2:uid="{2865FED8-1D15-40F6-8E78-7F59FD911D5F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Mata Pelajaran</t>
   </si>
@@ -50,6 +50,9 @@
   </si>
   <si>
     <t>Non KBM</t>
+  </si>
+  <si>
+    <t>Jatah Per Pekan</t>
   </si>
 </sst>
 </file>
@@ -151,11 +154,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}" name="Table1" displayName="Table1" ref="A1:B14" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:B14" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}"/>
-  <tableColumns count="2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}" name="Table1" displayName="Table1" ref="A1:C14" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C14" xr:uid="{90018943-7AD0-4845-8AC9-80DDA7D942A6}"/>
+  <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{7D525FBE-40AC-47DB-8530-6E9C3B2F11F5}" name="Kode Mapel" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{D1E7D42B-2E9F-491C-B453-3F034819E37D}" name="Jenis Mapel"/>
+    <tableColumn id="3" xr3:uid="{14FBEBDD-A97F-42FD-A4C0-02757F7F92FA}" name="Jatah Per Pekan"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -458,20 +462,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8C8015-952B-497B-B9AD-00108CB18956}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.28515625" style="3" customWidth="1"/>
     <col min="2" max="2" width="19.42578125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -479,6 +484,9 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>